<commit_message>
complete pin map spreadsheet
</commit_message>
<xml_diff>
--- a/Eagle 2018/pinout.xlsx
+++ b/Eagle 2018/pinout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
   <si>
     <t>Device</t>
   </si>
@@ -63,6 +63,279 @@
   </si>
   <si>
     <t>PA7</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Other Pin</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>TETHER_RX</t>
+  </si>
+  <si>
+    <t>TETHER_TX</t>
+  </si>
+  <si>
+    <t>BNO055</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>3VO</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>Explantion</t>
+  </si>
+  <si>
+    <t>output to tether</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> imput from tether</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>I2C Clock</t>
+  </si>
+  <si>
+    <t>I2C Data</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>3.3 Volts out</t>
+  </si>
+  <si>
+    <t>20 (SDA)</t>
+  </si>
+  <si>
+    <t>21 (SCL)</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>Changes I2C address from 0x28 to 0x29</t>
+  </si>
+  <si>
+    <t>MAX4312ESE</t>
+  </si>
+  <si>
+    <t>IN0</t>
+  </si>
+  <si>
+    <t>IN1</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>IN3</t>
+  </si>
+  <si>
+    <t>IN4</t>
+  </si>
+  <si>
+    <t>IN5</t>
+  </si>
+  <si>
+    <t>IN6</t>
+  </si>
+  <si>
+    <t>IN7</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>VIDEO_OUT</t>
+  </si>
+  <si>
+    <t>TETHER_VIDEO</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>VIDEO_0</t>
+  </si>
+  <si>
+    <t>VIDEO_1</t>
+  </si>
+  <si>
+    <t>VIDEO_2</t>
+  </si>
+  <si>
+    <t>VIDEO_3</t>
+  </si>
+  <si>
+    <t>VIDEO_4</t>
+  </si>
+  <si>
+    <t>VIDEO_5</t>
+  </si>
+  <si>
+    <t>VIDEO_6</t>
+  </si>
+  <si>
+    <t>VIDEO_7</t>
+  </si>
+  <si>
+    <t>Video Mux</t>
+  </si>
+  <si>
+    <t>Video Balun?</t>
+  </si>
+  <si>
+    <t>"+ in"</t>
+  </si>
+  <si>
+    <t>"- in"</t>
+  </si>
+  <si>
+    <t>"+ out"</t>
+  </si>
+  <si>
+    <t>"- out"</t>
+  </si>
+  <si>
+    <t>GND?</t>
+  </si>
+  <si>
+    <t>VIDEO_OUT?</t>
+  </si>
+  <si>
+    <t>ESCs</t>
+  </si>
+  <si>
+    <t>GND0</t>
+  </si>
+  <si>
+    <t>GND1</t>
+  </si>
+  <si>
+    <t>GND2</t>
+  </si>
+  <si>
+    <t>GND3</t>
+  </si>
+  <si>
+    <t>GND4</t>
+  </si>
+  <si>
+    <t>GND5</t>
+  </si>
+  <si>
+    <t>ESC_signal_0</t>
+  </si>
+  <si>
+    <t>ESC_signal_1</t>
+  </si>
+  <si>
+    <t>ESC_signal_2</t>
+  </si>
+  <si>
+    <t>ESC_signal_3</t>
+  </si>
+  <si>
+    <t>ESC_signal_4</t>
+  </si>
+  <si>
+    <t>ESC_signal_5</t>
+  </si>
+  <si>
+    <t>ESC_signal_6</t>
+  </si>
+  <si>
+    <t>ESC_signal_7</t>
+  </si>
+  <si>
+    <t>PE0</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>PG5</t>
+  </si>
+  <si>
+    <t>PH3</t>
+  </si>
+  <si>
+    <t>PH4</t>
+  </si>
+  <si>
+    <t>TX0</t>
+  </si>
+  <si>
+    <t>RX0</t>
+  </si>
+  <si>
+    <t>RS485 Receive Enable</t>
+  </si>
+  <si>
+    <t>RS485 Drive Enable</t>
+  </si>
+  <si>
+    <t>RS485 Drive Input</t>
+  </si>
+  <si>
+    <t>RS485 Receive Ouput</t>
+  </si>
+  <si>
+    <t>RS485 Vin</t>
   </si>
 </sst>
 </file>
@@ -417,21 +690,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4ACFCE-8431-423E-8CEA-EAAFDDE3D23D}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,60 +720,603 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D24" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="F24" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D25" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="1">
+        <v>25</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="1">
+        <v>26</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="1">
+        <v>27</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F48">
+    <sortCondition ref="A2:A48"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>